<commit_message>
add weekly demand value to input calculation
</commit_message>
<xml_diff>
--- a/spine_projects/01_input_data/01_input_raw/basic_input_calculations/demand_kasso_input_per_resolution.xlsx
+++ b/spine_projects/01_input_data/01_input_raw/basic_input_calculations/demand_kasso_input_per_resolution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\basic_input_calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7550BACB-1677-42D4-803E-6C4C0C16FA7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F98FB9-8805-47FD-A49B-5060081B8839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{4A53E8D8-29A5-45C6-8000-F5CF7751DA36}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{4A53E8D8-29A5-45C6-8000-F5CF7751DA36}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Demand</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>MWh</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>weeks/a</t>
   </si>
 </sst>
 </file>
@@ -494,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7BBB5B-23B4-4BB6-8FEB-C631920DB7D7}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -574,25 +580,34 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G6">
-        <v>12</v>
+        <f>365/7</f>
+        <v>52.142857142857146</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G7">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G9">
         <v>1</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H9" t="s">
         <v>18</v>
       </c>
     </row>
@@ -606,10 +621,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39F9F238-62E1-468B-A3E8-3469D0E1C6E4}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:I2"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -617,7 +632,7 @@
     <col min="4" max="4" width="17.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -634,13 +649,16 @@
         <v>12</v>
       </c>
       <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <f>Inputs!A2*Inputs!G2</f>
         <v>636800</v>
@@ -652,27 +670,31 @@
         <v>24</v>
       </c>
       <c r="E2">
+        <f>A3/Inputs!G9</f>
+        <v>176888.88888888888</v>
+      </c>
+      <c r="F2">
+        <f>Demand_calc!A3/Inputs!G8</f>
+        <v>44222.222222222219</v>
+      </c>
+      <c r="G2">
+        <f>A3/Inputs!G7</f>
+        <v>14740.740740740739</v>
+      </c>
+      <c r="H2">
         <f>A3/Inputs!G8</f>
-        <v>176888.88888888888</v>
-      </c>
-      <c r="F2">
-        <f>Demand_calc!A3/Inputs!G7</f>
         <v>44222.222222222219</v>
       </c>
-      <c r="G2">
-        <f>A3/Inputs!G6</f>
-        <v>14740.740740740739</v>
-      </c>
-      <c r="H2">
+      <c r="I2">
         <f>A3/Inputs!G5</f>
         <v>484.6270928462709</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <f>A3/Inputs!G4</f>
         <v>20.192795535261286</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <f>A2/Inputs!G3</f>
         <v>176888.88888888888</v>

</xml_diff>

<commit_message>
fix bug in demand calculation
</commit_message>
<xml_diff>
--- a/spine_projects/01_input_data/01_input_raw/basic_input_calculations/demand_kasso_input_per_resolution.xlsx
+++ b/spine_projects/01_input_data/01_input_raw/basic_input_calculations/demand_kasso_input_per_resolution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\basic_input_calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F98FB9-8805-47FD-A49B-5060081B8839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6C4DB6-577B-4EC1-8C82-FA6C68F18FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{4A53E8D8-29A5-45C6-8000-F5CF7751DA36}"/>
+    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{4A53E8D8-29A5-45C6-8000-F5CF7751DA36}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -624,7 +624,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="S34" sqref="S34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -682,8 +682,8 @@
         <v>14740.740740740739</v>
       </c>
       <c r="H2">
-        <f>A3/Inputs!G8</f>
-        <v>44222.222222222219</v>
+        <f>A3/Inputs!G6</f>
+        <v>3392.3896499238958</v>
       </c>
       <c r="I2">
         <f>A3/Inputs!G5</f>

</xml_diff>